<commit_message>
updating prices at 10:57:59
</commit_message>
<xml_diff>
--- a/script/modules/data/resources/constructor_prices.xlsx
+++ b/script/modules/data/resources/constructor_prices.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1195,6 +1195,41 @@
         <v>44042.83333333334</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="C22" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="G22" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="I22" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="J22" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>44042.91666666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updating prices at 11:31:01
</commit_message>
<xml_diff>
--- a/script/modules/data/resources/constructor_prices.xlsx
+++ b/script/modules/data/resources/constructor_prices.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,6 +1230,41 @@
         <v>44042.91666666666</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="B23" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E23" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="G23" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="I23" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="J23" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>44042.95833333334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>